<commit_message>
Added functionality to pass Adjacency tests
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ClueGame\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin Short\eclipse-workspace\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E3AAB-438D-4D8E-BC87-F32F5D7AEE06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055DA20A-E2FF-4389-9ED3-FA6280550001}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38772" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{773F7676-3B8C-4C7C-B85A-83C76B483AE4}"/>
+    <workbookView xWindow="-15885" yWindow="2415" windowWidth="15435" windowHeight="11835" xr2:uid="{773F7676-3B8C-4C7C-B85A-83C76B483AE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -605,37 +596,37 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" customWidth="1"/>
-    <col min="2" max="2" width="4.19921875" customWidth="1"/>
-    <col min="3" max="3" width="4.265625" customWidth="1"/>
-    <col min="4" max="4" width="5.19921875" customWidth="1"/>
-    <col min="5" max="5" width="5.265625" customWidth="1"/>
-    <col min="6" max="6" width="6.06640625" customWidth="1"/>
-    <col min="7" max="7" width="5.73046875" customWidth="1"/>
-    <col min="8" max="9" width="5.265625" customWidth="1"/>
-    <col min="10" max="10" width="5.53125" customWidth="1"/>
-    <col min="11" max="11" width="5.06640625" customWidth="1"/>
-    <col min="12" max="12" width="5.46484375" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
-    <col min="14" max="14" width="5.59765625" customWidth="1"/>
-    <col min="15" max="15" width="4.9296875" customWidth="1"/>
-    <col min="16" max="16" width="5.46484375" customWidth="1"/>
-    <col min="17" max="17" width="5.53125" customWidth="1"/>
-    <col min="18" max="18" width="4.86328125" customWidth="1"/>
-    <col min="19" max="19" width="3.9296875" customWidth="1"/>
-    <col min="20" max="20" width="4.1328125" customWidth="1"/>
-    <col min="21" max="21" width="4.53125" customWidth="1"/>
-    <col min="22" max="22" width="5.3984375" customWidth="1"/>
-    <col min="23" max="23" width="5.265625" customWidth="1"/>
-    <col min="27" max="27" width="50.46484375" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" customWidth="1"/>
+    <col min="18" max="18" width="4.85546875" customWidth="1"/>
+    <col min="19" max="19" width="4" customWidth="1"/>
+    <col min="20" max="20" width="4.140625" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" customWidth="1"/>
+    <col min="22" max="22" width="5.42578125" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" customWidth="1"/>
+    <col min="27" max="27" width="50.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>0</v>
       </c>
@@ -709,7 +700,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -786,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -863,7 +854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -937,7 +928,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1014,7 +1005,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1091,7 +1082,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1168,7 +1159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1245,7 +1236,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1319,7 +1310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1393,7 +1384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1467,7 +1458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1541,7 +1532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1615,7 +1606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1763,7 +1754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1837,7 +1828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1911,7 +1902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1985,7 +1976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2059,7 +2050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2133,7 +2124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2207,7 +2198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2281,7 +2272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2355,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2429,7 +2420,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2503,7 +2494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2577,7 +2568,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>

</xml_diff>